<commit_message>
added neg signals in python script and corrections on excel file
</commit_message>
<xml_diff>
--- a/vhdl_gen/lab2_MBE32bit.xlsx
+++ b/vhdl_gen/lab2_MBE32bit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anto\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anto\Documents\GitHub\isa16_lab2\vhdl_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E14763-AFE9-4698-A4D4-CCF7848EB831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36142609-210E-4540-BD0F-1981BE09ADDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15315" yWindow="990" windowWidth="21600" windowHeight="11385" xr2:uid="{1F6B4141-CC5C-4F94-8705-540E174ACDCF}"/>
+    <workbookView xWindow="7200" yWindow="3285" windowWidth="21600" windowHeight="11385" xr2:uid="{1F6B4141-CC5C-4F94-8705-540E174ACDCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -630,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -728,18 +728,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -761,14 +749,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1117,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739743BD-0E76-4192-9D50-6BAB97E2D3AD}">
   <dimension ref="K5:CF73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V72" sqref="V72"/>
+    <sheetView tabSelected="1" topLeftCell="BA49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BP70" sqref="BP70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,10 +1333,10 @@
       <c r="AX8" s="31"/>
     </row>
     <row r="9" spans="13:84" x14ac:dyDescent="0.25">
-      <c r="Q9" s="33" t="s">
+      <c r="Q9" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="AL9" s="43"/>
+      <c r="AL9" s="39"/>
       <c r="AU9" s="9" t="s">
         <v>1</v>
       </c>
@@ -1450,7 +1447,7 @@
       </c>
     </row>
     <row r="10" spans="13:84" x14ac:dyDescent="0.25">
-      <c r="Q10" s="33"/>
+      <c r="Q10" s="42"/>
       <c r="AT10" s="11">
         <v>1</v>
       </c>
@@ -1561,7 +1558,7 @@
       </c>
     </row>
     <row r="11" spans="13:84" x14ac:dyDescent="0.25">
-      <c r="Q11" s="33"/>
+      <c r="Q11" s="42"/>
       <c r="AR11" s="11">
         <v>1</v>
       </c>
@@ -1672,7 +1669,7 @@
       </c>
     </row>
     <row r="12" spans="13:84" x14ac:dyDescent="0.25">
-      <c r="Q12" s="33"/>
+      <c r="Q12" s="42"/>
       <c r="AP12" s="11">
         <v>1</v>
       </c>
@@ -1783,13 +1780,13 @@
       </c>
     </row>
     <row r="13" spans="13:84" x14ac:dyDescent="0.25">
-      <c r="M13" s="34" t="s">
+      <c r="M13" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="N13" s="35" t="s">
+      <c r="N13" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="Q13" s="33"/>
+      <c r="Q13" s="42"/>
       <c r="AN13" s="16">
         <v>1</v>
       </c>
@@ -1900,9 +1897,9 @@
       </c>
     </row>
     <row r="14" spans="13:84" x14ac:dyDescent="0.25">
-      <c r="M14" s="34"/>
-      <c r="N14" s="35"/>
-      <c r="Q14" s="33"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="44"/>
+      <c r="Q14" s="42"/>
       <c r="AL14" s="1">
         <v>1</v>
       </c>
@@ -2013,8 +2010,8 @@
       </c>
     </row>
     <row r="15" spans="13:84" x14ac:dyDescent="0.25">
-      <c r="M15" s="34"/>
-      <c r="Q15" s="33"/>
+      <c r="M15" s="43"/>
+      <c r="Q15" s="42"/>
       <c r="Z15" s="4"/>
       <c r="AJ15" s="1">
         <v>1</v>
@@ -2126,7 +2123,7 @@
       </c>
     </row>
     <row r="16" spans="13:84" x14ac:dyDescent="0.25">
-      <c r="Q16" s="33"/>
+      <c r="Q16" s="42"/>
       <c r="AH16" s="1">
         <v>1</v>
       </c>
@@ -2237,12 +2234,12 @@
       </c>
     </row>
     <row r="17" spans="13:82" x14ac:dyDescent="0.25">
-      <c r="M17" s="36" t="s">
+      <c r="M17" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="Q17" s="33"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="45"/>
+      <c r="Q17" s="42"/>
       <c r="AF17" s="1">
         <v>1</v>
       </c>
@@ -2353,10 +2350,10 @@
       </c>
     </row>
     <row r="18" spans="13:82" x14ac:dyDescent="0.25">
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="Q18" s="33"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="45"/>
+      <c r="Q18" s="42"/>
       <c r="AD18" s="1">
         <v>1</v>
       </c>
@@ -2467,10 +2464,10 @@
       </c>
     </row>
     <row r="19" spans="13:82" x14ac:dyDescent="0.25">
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="Q19" s="33"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="45"/>
+      <c r="Q19" s="42"/>
       <c r="AB19" s="1">
         <v>1</v>
       </c>
@@ -2581,10 +2578,10 @@
       </c>
     </row>
     <row r="20" spans="13:82" x14ac:dyDescent="0.25">
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="Q20" s="33"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="45"/>
+      <c r="Q20" s="42"/>
       <c r="Z20" s="1">
         <v>1</v>
       </c>
@@ -2695,7 +2692,7 @@
       </c>
     </row>
     <row r="21" spans="13:82" x14ac:dyDescent="0.25">
-      <c r="Q21" s="33"/>
+      <c r="Q21" s="42"/>
       <c r="X21" s="1">
         <v>1</v>
       </c>
@@ -2806,7 +2803,7 @@
       </c>
     </row>
     <row r="22" spans="13:82" x14ac:dyDescent="0.25">
-      <c r="Q22" s="33"/>
+      <c r="Q22" s="42"/>
       <c r="V22" s="19">
         <v>1</v>
       </c>
@@ -2918,7 +2915,7 @@
       </c>
     </row>
     <row r="23" spans="13:82" x14ac:dyDescent="0.25">
-      <c r="Q23" s="33"/>
+      <c r="Q23" s="42"/>
       <c r="T23" s="19">
         <v>1</v>
       </c>
@@ -3035,7 +3032,7 @@
       <c r="P24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q24" s="33"/>
+      <c r="Q24" s="42"/>
       <c r="S24" s="21" t="s">
         <v>16</v>
       </c>
@@ -3149,7 +3146,7 @@
       <c r="P25" s="1">
         <v>12</v>
       </c>
-      <c r="Q25" s="33"/>
+      <c r="Q25" s="42"/>
       <c r="S25" s="20" t="s">
         <v>0</v>
       </c>
@@ -3319,67 +3316,67 @@
       <c r="CD26" s="18"/>
     </row>
     <row r="27" spans="13:82" x14ac:dyDescent="0.25">
-      <c r="Q27" s="33" t="s">
+      <c r="Q27" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="AM27" s="40" t="s">
+      <c r="AM27" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="AN27" s="40" t="s">
+      <c r="AN27" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="AO27" s="40" t="s">
+      <c r="AO27" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="AP27" s="40" t="s">
+      <c r="AP27" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="AQ27" s="40" t="s">
+      <c r="AQ27" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="AR27" s="40" t="s">
+      <c r="AR27" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="AS27" s="40" t="s">
+      <c r="AS27" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="AT27" s="40" t="s">
+      <c r="AT27" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="AU27" s="40" t="s">
+      <c r="AU27" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="AV27" s="40" t="s">
+      <c r="AV27" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="AW27" s="40" t="s">
+      <c r="AW27" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="AX27" s="40" t="s">
+      <c r="AX27" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="AY27" s="40" t="s">
+      <c r="AY27" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="AZ27" s="40" t="s">
+      <c r="AZ27" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="BA27" s="40" t="s">
+      <c r="BA27" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="BB27" s="40" t="s">
+      <c r="BB27" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="BC27" s="40" t="s">
+      <c r="BC27" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="BD27" s="40" t="s">
+      <c r="BD27" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="BE27" s="40" t="s">
+      <c r="BE27" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="BF27" s="37" t="s">
+      <c r="BF27" s="33" t="s">
         <v>31</v>
       </c>
       <c r="BG27" s="5" t="s">
@@ -3456,65 +3453,65 @@
       </c>
     </row>
     <row r="28" spans="13:82" x14ac:dyDescent="0.25">
-      <c r="Q28" s="33"/>
+      <c r="Q28" s="42"/>
       <c r="AL28" s="11">
         <v>1</v>
       </c>
-      <c r="AM28" s="44" t="s">
+      <c r="AM28" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AN28" s="38" t="s">
+      <c r="AN28" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="AO28" s="41" t="s">
+      <c r="AO28" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="AP28" s="41" t="s">
+      <c r="AP28" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="AQ28" s="41" t="s">
+      <c r="AQ28" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="AR28" s="41" t="s">
+      <c r="AR28" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="AS28" s="41" t="s">
+      <c r="AS28" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="AT28" s="41" t="s">
+      <c r="AT28" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="AU28" s="41" t="s">
+      <c r="AU28" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="AV28" s="41" t="s">
+      <c r="AV28" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="AW28" s="41" t="s">
+      <c r="AW28" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="AX28" s="41" t="s">
+      <c r="AX28" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="AY28" s="41" t="s">
+      <c r="AY28" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="AZ28" s="41" t="s">
+      <c r="AZ28" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="BA28" s="41" t="s">
+      <c r="BA28" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="BB28" s="41" t="s">
+      <c r="BB28" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="BC28" s="41" t="s">
+      <c r="BC28" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="BD28" s="38" t="s">
+      <c r="BD28" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="BE28" s="38" t="s">
+      <c r="BE28" s="34" t="s">
         <v>33</v>
       </c>
       <c r="BF28" s="8" t="s">
@@ -3591,7 +3588,7 @@
       </c>
     </row>
     <row r="29" spans="13:82" x14ac:dyDescent="0.25">
-      <c r="Q29" s="33"/>
+      <c r="Q29" s="42"/>
       <c r="AJ29" s="11">
         <v>1</v>
       </c>
@@ -3607,52 +3604,52 @@
       <c r="AN29" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="AO29" s="39" t="s">
+      <c r="AO29" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="AP29" s="39" t="s">
+      <c r="AP29" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="AQ29" s="42" t="s">
+      <c r="AQ29" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="AR29" s="42" t="s">
+      <c r="AR29" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="AS29" s="42" t="s">
+      <c r="AS29" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="AT29" s="42" t="s">
+      <c r="AT29" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="AU29" s="42" t="s">
+      <c r="AU29" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="AV29" s="42" t="s">
+      <c r="AV29" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="AW29" s="42" t="s">
+      <c r="AW29" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="AX29" s="42" t="s">
+      <c r="AX29" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="AY29" s="42" t="s">
+      <c r="AY29" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="AZ29" s="42" t="s">
+      <c r="AZ29" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="BA29" s="41" t="s">
+      <c r="BA29" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="BB29" s="39" t="s">
+      <c r="BB29" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="BC29" s="39" t="s">
+      <c r="BC29" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="BD29" s="39" t="s">
+      <c r="BD29" s="35" t="s">
         <v>36</v>
       </c>
       <c r="BE29" s="6" t="s">
@@ -3726,7 +3723,7 @@
       </c>
     </row>
     <row r="30" spans="13:82" x14ac:dyDescent="0.25">
-      <c r="Q30" s="33"/>
+      <c r="Q30" s="42"/>
       <c r="AH30" s="11">
         <v>1</v>
       </c>
@@ -3751,46 +3748,46 @@
       <c r="AO30" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AP30" s="37" t="s">
+      <c r="AP30" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="AQ30" s="37" t="s">
+      <c r="AQ30" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="AR30" s="37" t="s">
+      <c r="AR30" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="AS30" s="40" t="s">
+      <c r="AS30" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="AT30" s="40" t="s">
+      <c r="AT30" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="AU30" s="40" t="s">
+      <c r="AU30" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="AV30" s="40" t="s">
+      <c r="AV30" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="AW30" s="40" t="s">
+      <c r="AW30" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="AX30" s="40" t="s">
+      <c r="AX30" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="AY30" s="40" t="s">
+      <c r="AY30" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="AZ30" s="37" t="s">
+      <c r="AZ30" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="BA30" s="37" t="s">
+      <c r="BA30" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="BB30" s="37" t="s">
+      <c r="BB30" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="BC30" s="37" t="s">
+      <c r="BC30" s="33" t="s">
         <v>40</v>
       </c>
       <c r="BD30" s="5" t="s">
@@ -3861,7 +3858,7 @@
       </c>
     </row>
     <row r="31" spans="13:82" x14ac:dyDescent="0.25">
-      <c r="Q31" s="33"/>
+      <c r="Q31" s="42"/>
       <c r="AF31" s="16">
         <v>1</v>
       </c>
@@ -3895,40 +3892,40 @@
       <c r="AP31" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="AQ31" s="38" t="s">
+      <c r="AQ31" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="AR31" s="38" t="s">
+      <c r="AR31" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="AS31" s="38" t="s">
+      <c r="AS31" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="AT31" s="38" t="s">
+      <c r="AT31" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="AU31" s="38" t="s">
+      <c r="AU31" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="AV31" s="38" t="s">
+      <c r="AV31" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="AW31" s="38" t="s">
+      <c r="AW31" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="AX31" s="38" t="s">
+      <c r="AX31" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="AY31" s="38" t="s">
+      <c r="AY31" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="AZ31" s="38" t="s">
+      <c r="AZ31" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="BA31" s="38" t="s">
+      <c r="BA31" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="BB31" s="38" t="s">
+      <c r="BB31" s="34" t="s">
         <v>45</v>
       </c>
       <c r="BC31" s="8" t="s">
@@ -3996,7 +3993,7 @@
       </c>
     </row>
     <row r="32" spans="13:82" x14ac:dyDescent="0.25">
-      <c r="Q32" s="33"/>
+      <c r="Q32" s="42"/>
       <c r="AD32" s="1">
         <v>1</v>
       </c>
@@ -4039,34 +4036,34 @@
       <c r="AQ32" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="AR32" s="39" t="s">
+      <c r="AR32" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="AS32" s="39" t="s">
+      <c r="AS32" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="AT32" s="39" t="s">
+      <c r="AT32" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="AU32" s="39" t="s">
+      <c r="AU32" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="AV32" s="39" t="s">
+      <c r="AV32" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="AW32" s="39" t="s">
+      <c r="AW32" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="AX32" s="39" t="s">
+      <c r="AX32" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="AY32" s="39" t="s">
+      <c r="AY32" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="AZ32" s="39" t="s">
+      <c r="AZ32" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="BA32" s="39" t="s">
+      <c r="BA32" s="35" t="s">
         <v>51</v>
       </c>
       <c r="BB32" s="6" t="s">
@@ -4131,7 +4128,7 @@
       </c>
     </row>
     <row r="33" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q33" s="33"/>
+      <c r="Q33" s="42"/>
       <c r="AB33" s="1">
         <v>1</v>
       </c>
@@ -4183,28 +4180,28 @@
       <c r="AR33" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AS33" s="37" t="s">
+      <c r="AS33" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="AT33" s="37" t="s">
+      <c r="AT33" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="AU33" s="37" t="s">
+      <c r="AU33" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="AV33" s="37" t="s">
+      <c r="AV33" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="AW33" s="37" t="s">
+      <c r="AW33" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="AX33" s="37" t="s">
+      <c r="AX33" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="AY33" s="37" t="s">
+      <c r="AY33" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="AZ33" s="37" t="s">
+      <c r="AZ33" s="33" t="s">
         <v>58</v>
       </c>
       <c r="BA33" s="5" t="s">
@@ -4266,7 +4263,7 @@
       </c>
     </row>
     <row r="34" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q34" s="33"/>
+      <c r="Q34" s="42"/>
       <c r="Z34" s="1">
         <v>1</v>
       </c>
@@ -4327,22 +4324,22 @@
       <c r="AS34" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="AT34" s="38" t="s">
+      <c r="AT34" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="AU34" s="38" t="s">
+      <c r="AU34" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="AV34" s="38" t="s">
+      <c r="AV34" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="AW34" s="38" t="s">
+      <c r="AW34" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="AX34" s="38" t="s">
+      <c r="AX34" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="AY34" s="38" t="s">
+      <c r="AY34" s="34" t="s">
         <v>66</v>
       </c>
       <c r="AZ34" s="8" t="s">
@@ -4401,7 +4398,7 @@
       </c>
     </row>
     <row r="35" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q35" s="33"/>
+      <c r="Q35" s="42"/>
       <c r="X35" s="1">
         <v>1</v>
       </c>
@@ -4536,7 +4533,7 @@
       </c>
     </row>
     <row r="36" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q36" s="33"/>
+      <c r="Q36" s="42"/>
       <c r="V36" s="19">
         <v>1</v>
       </c>
@@ -4672,7 +4669,7 @@
       </c>
     </row>
     <row r="37" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q37" s="33"/>
+      <c r="Q37" s="42"/>
       <c r="T37" s="19">
         <v>1</v>
       </c>
@@ -4813,7 +4810,7 @@
       <c r="P38" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q38" s="33"/>
+      <c r="Q38" s="42"/>
       <c r="S38" s="21" t="s">
         <v>16</v>
       </c>
@@ -4951,7 +4948,7 @@
       <c r="P39" s="1">
         <v>12</v>
       </c>
-      <c r="Q39" s="33"/>
+      <c r="Q39" s="42"/>
       <c r="S39" s="20" t="s">
         <v>0</v>
       </c>
@@ -5144,7 +5141,7 @@
       <c r="CD40" s="18"/>
     </row>
     <row r="41" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q41" s="33" t="s">
+      <c r="Q41" s="42" t="s">
         <v>21</v>
       </c>
       <c r="AE41" s="5" t="s">
@@ -5305,7 +5302,7 @@
       </c>
     </row>
     <row r="42" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q42" s="33"/>
+      <c r="Q42" s="42"/>
       <c r="AD42" s="11">
         <v>1</v>
       </c>
@@ -5464,7 +5461,7 @@
       </c>
     </row>
     <row r="43" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q43" s="33"/>
+      <c r="Q43" s="42"/>
       <c r="AB43" s="11">
         <v>1</v>
       </c>
@@ -5623,7 +5620,7 @@
       </c>
     </row>
     <row r="44" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q44" s="33"/>
+      <c r="Q44" s="42"/>
       <c r="Z44" s="16">
         <v>1</v>
       </c>
@@ -5782,7 +5779,7 @@
       </c>
     </row>
     <row r="45" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q45" s="33"/>
+      <c r="Q45" s="42"/>
       <c r="S45" s="22"/>
       <c r="T45" s="22"/>
       <c r="U45" s="22"/>
@@ -5946,7 +5943,7 @@
       </c>
     </row>
     <row r="46" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q46" s="33"/>
+      <c r="Q46" s="42"/>
       <c r="S46" s="22"/>
       <c r="T46" s="22"/>
       <c r="U46" s="22"/>
@@ -6108,7 +6105,7 @@
       </c>
     </row>
     <row r="47" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q47" s="33"/>
+      <c r="Q47" s="42"/>
       <c r="S47" s="22"/>
       <c r="T47" s="19">
         <v>1</v>
@@ -6275,7 +6272,7 @@
       <c r="P48" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q48" s="33"/>
+      <c r="Q48" s="42"/>
       <c r="S48" s="21" t="s">
         <v>16</v>
       </c>
@@ -6437,7 +6434,7 @@
       <c r="P49" s="1">
         <v>9</v>
       </c>
-      <c r="Q49" s="33"/>
+      <c r="Q49" s="42"/>
       <c r="S49" s="20" t="s">
         <v>0</v>
       </c>
@@ -6655,7 +6652,7 @@
       <c r="CD50" s="18"/>
     </row>
     <row r="51" spans="11:82" x14ac:dyDescent="0.25">
-      <c r="Q51" s="33" t="s">
+      <c r="Q51" s="42" t="s">
         <v>22</v>
       </c>
       <c r="S51" s="22"/>
@@ -6840,13 +6837,13 @@
       </c>
     </row>
     <row r="52" spans="11:82" x14ac:dyDescent="0.25">
-      <c r="Q52" s="33"/>
+      <c r="Q52" s="42"/>
       <c r="S52" s="22"/>
       <c r="T52" s="22"/>
       <c r="U52" s="22"/>
       <c r="V52" s="22"/>
       <c r="W52" s="22"/>
-      <c r="X52" s="45">
+      <c r="X52" s="40">
         <v>1</v>
       </c>
       <c r="Y52" s="10" t="s">
@@ -7022,11 +7019,11 @@
       </c>
     </row>
     <row r="53" spans="11:82" x14ac:dyDescent="0.25">
-      <c r="Q53" s="33"/>
+      <c r="Q53" s="42"/>
       <c r="S53" s="22"/>
       <c r="T53" s="22"/>
       <c r="U53" s="22"/>
-      <c r="V53" s="46">
+      <c r="V53" s="41">
         <v>1</v>
       </c>
       <c r="W53" s="9" t="s">
@@ -7202,7 +7199,7 @@
       </c>
     </row>
     <row r="54" spans="11:82" x14ac:dyDescent="0.25">
-      <c r="Q54" s="33"/>
+      <c r="Q54" s="42"/>
       <c r="S54" s="22"/>
       <c r="T54" s="22">
         <v>1</v>
@@ -7386,7 +7383,7 @@
       <c r="P55" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q55" s="33"/>
+      <c r="Q55" s="42"/>
       <c r="S55" s="21" t="s">
         <v>16</v>
       </c>
@@ -7567,7 +7564,7 @@
       <c r="P56" s="1">
         <v>6</v>
       </c>
-      <c r="Q56" s="33"/>
+      <c r="Q56" s="42"/>
       <c r="S56" s="20" t="s">
         <v>0</v>
       </c>
@@ -7804,7 +7801,7 @@
       <c r="CD57" s="18"/>
     </row>
     <row r="58" spans="11:82" x14ac:dyDescent="0.25">
-      <c r="Q58" s="33" t="s">
+      <c r="Q58" s="42" t="s">
         <v>24</v>
       </c>
       <c r="U58" s="5" t="s">
@@ -7996,7 +7993,7 @@
     </row>
     <row r="59" spans="11:82" x14ac:dyDescent="0.25">
       <c r="K59" s="2"/>
-      <c r="Q59" s="33"/>
+      <c r="Q59" s="42"/>
       <c r="S59" s="22"/>
       <c r="T59" s="16">
         <v>1</v>
@@ -8192,7 +8189,7 @@
       <c r="P60" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q60" s="33"/>
+      <c r="Q60" s="42"/>
       <c r="S60" s="24" t="s">
         <v>16</v>
       </c>
@@ -8384,7 +8381,7 @@
       <c r="P61" s="1">
         <v>3</v>
       </c>
-      <c r="Q61" s="33"/>
+      <c r="Q61" s="42"/>
       <c r="S61" s="20" t="s">
         <v>0</v>
       </c>
@@ -8631,7 +8628,7 @@
       <c r="CD62" s="18"/>
     </row>
     <row r="63" spans="11:82" x14ac:dyDescent="0.25">
-      <c r="Q63" s="33" t="s">
+      <c r="Q63" s="42" t="s">
         <v>23</v>
       </c>
       <c r="S63" s="5" t="s">
@@ -8834,7 +8831,7 @@
       <c r="P64" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q64" s="33"/>
+      <c r="Q64" s="42"/>
       <c r="S64" s="10" t="s">
         <v>16</v>
       </c>
@@ -9032,7 +9029,7 @@
       <c r="P65" s="1">
         <v>2</v>
       </c>
-      <c r="Q65" s="33"/>
+      <c r="Q65" s="42"/>
       <c r="S65" s="6" t="s">
         <v>0</v>
       </c>
@@ -9286,7 +9283,7 @@
       <c r="CD66" s="18"/>
     </row>
     <row r="67" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q67" s="33" t="s">
+      <c r="Q67" s="42" t="s">
         <v>25</v>
       </c>
       <c r="R67" s="3" t="s">
@@ -9486,7 +9483,7 @@
       </c>
     </row>
     <row r="68" spans="15:82" x14ac:dyDescent="0.25">
-      <c r="Q68" s="33"/>
+      <c r="Q68" s="42"/>
       <c r="S68" s="3" t="s">
         <v>0</v>
       </c>
@@ -9673,7 +9670,7 @@
       <c r="CB68" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="CC68" s="4">
+      <c r="CC68" s="2">
         <v>0</v>
       </c>
       <c r="CD68" s="1" t="s">
@@ -9690,6 +9687,7 @@
       <c r="P70" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="BP70" s="2"/>
     </row>
     <row r="71" spans="15:82" x14ac:dyDescent="0.25">
       <c r="O71" s="1">

</xml_diff>

<commit_message>
added pp_gen on python script
</commit_message>
<xml_diff>
--- a/vhdl_gen/lab2_MBE32bit.xlsx
+++ b/vhdl_gen/lab2_MBE32bit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anto\Documents\GitHub\isa16_lab2\vhdl_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36142609-210E-4540-BD0F-1981BE09ADDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5ECD7D-0DCB-4287-988A-EF4F120481D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3285" windowWidth="21600" windowHeight="11385" xr2:uid="{1F6B4141-CC5C-4F94-8705-540E174ACDCF}"/>
+    <workbookView xWindow="7200" yWindow="2565" windowWidth="21600" windowHeight="11385" xr2:uid="{1F6B4141-CC5C-4F94-8705-540E174ACDCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -630,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -766,6 +766,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1114,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739743BD-0E76-4192-9D50-6BAB97E2D3AD}">
   <dimension ref="K5:CF73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BP70" sqref="BP70"/>
+    <sheetView tabSelected="1" topLeftCell="O43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S68" sqref="S68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9667,7 +9670,7 @@
       <c r="CA68" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="CB68" s="24" t="s">
+      <c r="CB68" s="46" t="s">
         <v>2</v>
       </c>
       <c r="CC68" s="2">

</xml_diff>